<commit_message>
changed output details and changed to use pathlib
</commit_message>
<xml_diff>
--- a/outputs/configuration.xlsx
+++ b/outputs/configuration.xlsx
@@ -7,9 +7,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="interfaces" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="firewall_objects" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="interfaces" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="address-objects" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="firewall-addrgrp" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="service-custom" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="service-group" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="firewall-policy" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="router-static" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,24 +431,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1361,7 +1347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1413,9 +1399,6 @@
           <t>"all"</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1428,9 +1411,6 @@
           <t>"FIREWALL_AUTH_PORTAL_ADDRESS"</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1443,9 +1423,6 @@
           <t>"FABRIC_DEVICE"</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1468,7 +1445,6 @@
           <t>iprange</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1481,13 +1457,11 @@
           <t>"FCTEMS_ALL_FORTICLOUD_SERVERS"</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>dynamic</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1500,8 +1474,6 @@
           <t>"nw-ap01"</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>192.168.7.10 255.255.255.255</t>
@@ -1519,8 +1491,6 @@
           <t>"nw-ap02"</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>192.168.7.11 255.255.255.255</t>
@@ -1538,8 +1508,6 @@
           <t>"nw-ap03"</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>192.168.7.13 255.255.255.255</t>
@@ -1557,8 +1525,6 @@
           <t>"nw-ap04"</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>192.168.7.14 255.255.255.255</t>
@@ -1576,8 +1542,6 @@
           <t>"nw-ap05"</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
           <t>192.168.7.15 255.255.255.255</t>
@@ -1595,8 +1559,6 @@
           <t>"nw-ap06"</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>192.168.7.16 255.255.255.255</t>
@@ -1614,11 +1576,1650 @@
           <t>"nw-ap07"</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
           <t>192.168.7.17 255.255.255.255</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>members</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>uudi</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>"Private RFC1918 10.0.0.0" "Private RFC1918 172.16.0.0" "Private RFC1918 192.168.0.0" "Private RFC6598 100.64.0.0"</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>"Private Address Spaces"</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>"NetSG AU01 Mgmt DMZ Subnet" "NetSG AU02 Mgmt DMZ Subnet"</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>3d04fc60-c17f-51ec-0e13-e7a73304a5ed</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>"NetSG Mgmt DMZ Subnets"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>"NetSG NTP Server 1" "NetSG NTP Server 2"</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>52ed8bdc-c17f-51ec-8732-eb6bb4f3e18c</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>"NetSG NTP Servers"</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>"NetSG Tacacs Server 1" "NetSG Tacacs Server 2"</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>602507bc-c17f-51ec-b284-494cdbd261c2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"NetSG Tacacs Servers"</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>"nw-ap01" "nw-ap02" "nw-ap03" "nw-ap04" "nw-ap05" "nw-ap06" "nw-ap07"</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3e2be308-e87e-51ec-ecb0-49a688dc1ce9</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>"Baulkham Hills Meraki APs"</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>udp-portrange</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>tcp-portrange</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>proxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>"DNS"</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>"HTTP"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>"HTTPS"</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>143</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"IMAP"</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>"Email"</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>993</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>"IMAPS"</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>"Email"</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>389</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>"LDAP"</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>"Authentication"</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>"DCE-RPC"</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>"POP3"</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>"Email"</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>995</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>"POP3S"</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>"Email"</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>139</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>"SAMBA"</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>"SMTP"</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>"Email"</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>465</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>"SMTPS"</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>"Email"</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>"KERBEROS"</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>"Authentication"</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>389</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>"LDAP_UDP"</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>"Authentication"</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>445</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>"SMB"</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>"ALL"</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>"General"</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>IP</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>"ALL_ICMP"</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>"General"</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>ICMP</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>"NTP"</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>"PING"</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ICMP</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>161-162</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>161-162</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>"SNMP"</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>"SSH"</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>33434-33535</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>"TRACEROUTE"</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0-65535:0-65535</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>"webproxy"</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ALL</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>4433</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>"FortiGateAdminPort"</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>"TACACS+"</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>"udp-443"</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>8080</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>"tcp-8080"</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>member</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>"DNS" "IMAP" "IMAPS" "POP3" "POP3S" "SMTP" "SMTPS"</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>"Email Access"</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>"DNS" "HTTP" "HTTPS"</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"Web Access"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>"DCE-RPC" "DNS" "KERBEROS" "LDAP" "LDAP_UDP" "SAMBA" "SMB"</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"Windows AD"</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>"DCE-RPC" "DNS" "HTTPS"</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"Exchange Server"</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>logtraffic</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>schedule</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>action</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dstaddr</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>srcaddr</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>dstintf</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>srcintf</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>uuid</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>nat</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ssl-ssh-profile</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>utm-status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>"ALL_ICMP" "FortiGateAdminPort" "HTTPS" "SNMP" "SSH"</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>"NetSG SNCK Loopback Allocation"</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>"NetSG Mgmt DMZ Subnets"</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>"loopback0" "internal3"</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>"Zone_IPWan"</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>652c632c-c23d-51ec-9b0c-366b86d43aa6</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>"NetSG Management Inbound"</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>"NTP"</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>"NetSG NTP Servers"</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>"NetSG SNCK Loopback Allocation"</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>"Zone_IPWan"</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>"loopback0"</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>652fad48-c23d-51ec-b6f9-837c0a35e74b</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>"NetSG NTP Servers"</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>"TACACS+"</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>"NetSG Tacacs Servers"</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>"NetSG SNCK Loopback Allocation"</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>"Zone_IPWan"</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>"loopback0"</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>653036be-c23d-51ec-98c9-1e91fe7e21f6</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>"NetSG TACACS Servers"</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>"PING" "TRACEROUTE"</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>"Private Address Spaces"</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>"Private Address Spaces"</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>"any"</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>"any"</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>6530c480-c23d-51ec-65f0-49633702aa26</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>"Trusted Internal ICMP"</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>"ALL"</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>"Zone_IPWan"</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>"Zone_Data"</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>65314c98-c23d-51ec-3c19-dbed9849c03f</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>"LAN to IPWAN"</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>"ALL"</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>"Zone_Data"</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>"Zone_IPWan"</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>6531d5c8-c23d-51ec-38ed-d0fdd6ee45ba</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>"IPWAN to LAN"</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>"ALL"</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>"Private Address Spaces"</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>"virtual-wan-link"</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>"any"</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>4674fb24-e871-51ec-f6d9-123c05f4aa93</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>"Protect Internal"</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>"Meraki Ports" "PING" "NTP"</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>"Baulkham Hills Meraki APs"</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>"virtual-wan-link"</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>"Zone_Data"</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>476097d0-e87d-51ec-bf3a-e97a6bcbeef4</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>"Meraki Access Points"</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>"This is only additional ports required for Speedtest.net.</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>"certificate-inspection"</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>"udp-443" "tcp-8080"</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>"virtual-wan-link"</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>"Zone_Data"</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>95857f32-e870-51ec-38d8-9faf909dc008</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>"Speedtest Access"</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>"This is only additional ports required for Speedtest.net.</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>"certificate-inspection"</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>"ALL"</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>"virtual-wan-link"</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>"Zone_Data"</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>6532647a-c23d-51ec-afcf-59860ca87a75</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>"General Internet Access"</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>"certificate-inspection"</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>all</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>"ALL"</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>"always"</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>"all"</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>"any"</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>"any"</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>73129d2e-c645-51ec-7001-bbead48d8665</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>"Deny and Log"</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>blackhole</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>distance</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>dst</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>254</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10.0.0.0 255.0.0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>254</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>100.64.0.0 255.192.0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>254</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>172.16.0.0 255.240.0.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>254</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>192.168.0.0 255.255.0.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>192.168.6.0 255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>192.168.7.0 255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>103.99.241.36 255.255.255.255</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>103.99.241.35 255.255.255.255</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>103.99.243.129 255.255.255.255</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>103.99.241.10 255.255.255.255</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added some regex to the template and cleaning up some of the outputs to remove quotes and covert to list where appropriate
</commit_message>
<xml_diff>
--- a/outputs/configuration.xlsx
+++ b/outputs/configuration.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ping fgfm</t>
+          <t>['ping', 'fgfm']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>ping fgfm</t>
+          <t>['ping', 'fgfm']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -648,7 +648,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>ping https fgfm fabric</t>
+          <t>['ping', 'https', 'fgfm', 'fabric']</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>10.10.10.1 255.255.255.0</t>
+          <t>10.10.10.1/24</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>"To-LAN"</t>
+          <t>To-LAN</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>"To-LAN"</t>
+          <t>To-LAN</t>
         </is>
       </c>
     </row>
@@ -734,7 +734,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>ping https ssh http fgfm fabric</t>
+          <t>['ping', 'https', 'ssh', 'http', 'fgfm', 'fabric']</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -749,12 +749,12 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>100.64.24.237 255.255.255.252</t>
+          <t>100.64.24.237/30</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>"FortiExtender"</t>
+          <t>FortiExtender</t>
         </is>
       </c>
     </row>
@@ -923,7 +923,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>ping https ssh fgfm fabric</t>
+          <t>['ping', 'https', 'ssh', 'fgfm', 'fabric']</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>192.168.1.99 255.255.255.0</t>
+          <t>192.168.1.99/24</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>ping fabric</t>
+          <t>['ping', 'fabric']</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -980,7 +980,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>169.254.1.1 255.255.255.0</t>
+          <t>169.254.1.1/24</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>a" "b</t>
+          <t>['a', 'b']</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>ping https ssh snmp</t>
+          <t>['ping', 'https', 'ssh', 'snmp']</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1027,7 +1027,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>100.64.24.5 255.255.255.255</t>
+          <t>100.64.24.5/32</t>
         </is>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>100.66.11.22 255.255.255.252</t>
+          <t>100.66.11.22/30</t>
         </is>
       </c>
       <c r="R17" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>89.147.120.215 255.255.255.254</t>
+          <t>89.147.120.215/31</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1138,7 +1138,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>100.66.11.26 255.255.255.252</t>
+          <t>100.66.11.26/30</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>100.66.11.134 255.255.255.255</t>
+          <t>100.66.11.134/32</t>
         </is>
       </c>
     </row>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>100.66.11.166 255.255.255.255</t>
+          <t>100.66.11.166/32</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>192.168.5.1 255.255.255.0</t>
+          <t>192.168.5.1/24</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -1291,7 +1291,7 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>internal1" "internal2</t>
+          <t>['internal1', 'internal2']</t>
         </is>
       </c>
       <c r="R23" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ping</t>
+          <t>['ping']</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>89.147.120.213 255.255.255.254</t>
+          <t>89.147.120.213/31</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -1353,7 +1353,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1374,15 +1374,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>comment</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>end_ip</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>start_ip</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>associated-interface</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>subnet</t>
         </is>
@@ -1396,7 +1411,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>all</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1423,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>"FIREWALL_AUTH_PORTAL_ADDRESS"</t>
+          <t>FIREWALL_AUTH_PORTAL_ADDRESS</t>
         </is>
       </c>
     </row>
@@ -1420,7 +1435,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>"FABRIC_DEVICE"</t>
+          <t>FABRIC_DEVICE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>IPv4 addresses of Fabric Devices.</t>
         </is>
       </c>
     </row>
@@ -1432,15 +1452,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>"SSLVPN_TUNNEL_ADDR1"</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>"ssl.root"</t>
+          <t>SSLVPN_TUNNEL_ADDR1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
+        <is>
+          <t>10.212.134.210</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>10.212.134.200</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ssl.root</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>iprange</t>
         </is>
@@ -1454,10 +1484,10 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>"FCTEMS_ALL_FORTICLOUD_SERVERS"</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
+          <t>FCTEMS_ALL_FORTICLOUD_SERVERS</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>dynamic</t>
         </is>
@@ -1466,119 +1496,306 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ea5b02fe-e87d-51ec-45de-1058c8dc3015</t>
+          <t>9dd63474-c17e-51ec-414e-d391de278269</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>"nw-ap01"</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>192.168.7.10 255.255.255.255</t>
+          <t>Private RFC1918 10.0.0.0</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>10.0.0.0/8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>f55a2360-e87d-51ec-a5d9-f95c9392cb67</t>
+          <t>accc70ba-c17e-51ec-a150-34dd5295486c</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>"nw-ap02"</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>192.168.7.11 255.255.255.255</t>
+          <t>Private RFC1918 172.16.0.0</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>172.16.0.0/12</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>017a06d8-e87e-51ec-ab97-93410a582ec4</t>
+          <t>bacc7c8c-c17e-51ec-1b44-78ac0eaac98d</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>"nw-ap03"</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>192.168.7.13 255.255.255.255</t>
+          <t>Private RFC1918 192.168.0.0</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>192.168.0.0/16</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0ba7bf88-e87e-51ec-76cc-c7cc7b08155b</t>
+          <t>f4c6c104-c17e-51ec-79d7-995927036c68</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>"nw-ap04"</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>192.168.7.14 255.255.255.255</t>
+          <t>Private RFC6598 100.64.0.0</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>100.64.0.0/10</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17a955da-e87e-51ec-e257-f807bbfdb39b</t>
+          <t>7193e550-c17e-51ec-5133-435ce1ae000e</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>"nw-ap05"</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>192.168.7.15 255.255.255.255</t>
+          <t>NetSG AU01 Mgmt DMZ Subnet</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>100.68.1.0/24</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>265076fe-e87e-51ec-ecc0-4471a7f569c0</t>
+          <t>7e302878-c17e-51ec-2aaa-add873a5d0b5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>"nw-ap06"</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>192.168.7.16 255.255.255.255</t>
+          <t>NetSG AU02 Mgmt DMZ Subnet</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>100.68.2.0/24</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>061f6e06-c17f-51ec-9ace-68cf37c88867</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>NetSG NTP Server 1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>103.74.171.50/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>10262f7a-c17f-51ec-423e-2abd67c5a3e0</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>NetSG NTP Server 2</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>103.99.241.50/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>8f652b66-c17e-51ec-d179-d72dbd46e0e5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>NetSG SNCK Loopback Allocation</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>100.64.24.0/24</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>19948d0e-c17f-51ec-208d-651c24467a49</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>NetSG Tacacs Server 1</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>100.68.1.133/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2353eaf6-c17f-51ec-935d-653521fb65a3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>NetSG Tacacs Server 2</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>100.68.2.133/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ea5b02fe-e87d-51ec-45de-1058c8dc3015</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>nw-ap01</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>192.168.7.10/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>f55a2360-e87d-51ec-a5d9-f95c9392cb67</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>nw-ap02</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>192.168.7.11/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>017a06d8-e87e-51ec-ab97-93410a582ec4</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>nw-ap03</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>192.168.7.13/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0ba7bf88-e87e-51ec-76cc-c7cc7b08155b</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>nw-ap04</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>192.168.7.14/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>17a955da-e87e-51ec-e257-f807bbfdb39b</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>nw-ap05</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>192.168.7.15/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>265076fe-e87e-51ec-ecc0-4471a7f569c0</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>nw-ap06</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>192.168.7.16/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>2e109428-e87e-51ec-6083-96f05f3296af</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>"nw-ap07"</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>192.168.7.17 255.255.255.255</t>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>nw-ap07</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>192.168.7.17/32</t>
         </is>
       </c>
     </row>
@@ -1621,7 +1838,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"Private RFC1918 10.0.0.0" "Private RFC1918 172.16.0.0" "Private RFC1918 192.168.0.0" "Private RFC6598 100.64.0.0"</t>
+          <t>['Private', 'RFC1918', '10.0.0.0', 'Private', 'RFC1918', '172.16.0.0', 'Private', 'RFC1918', '192.168.0.0', 'Private', 'RFC6598', '100.64.0.0']</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1631,14 +1848,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"Private Address Spaces"</t>
+          <t>Private Address Spaces</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"NetSG AU01 Mgmt DMZ Subnet" "NetSG AU02 Mgmt DMZ Subnet"</t>
+          <t>['NetSG', 'AU01', 'Mgmt', 'DMZ', 'Subnet', 'NetSG', 'AU02', 'Mgmt', 'DMZ', 'Subnet']</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1648,14 +1865,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"NetSG Mgmt DMZ Subnets"</t>
+          <t>NetSG Mgmt DMZ Subnets</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"NetSG NTP Server 1" "NetSG NTP Server 2"</t>
+          <t>['NetSG', 'NTP', 'Server', '1', 'NetSG', 'NTP', 'Server', '2']</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1665,14 +1882,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"NetSG NTP Servers"</t>
+          <t>NetSG NTP Servers</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"NetSG Tacacs Server 1" "NetSG Tacacs Server 2"</t>
+          <t>['NetSG', 'Tacacs', 'Server', '1', 'NetSG', 'Tacacs', 'Server', '2']</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1682,14 +1899,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"NetSG Tacacs Servers"</t>
+          <t>NetSG Tacacs Servers</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>"nw-ap01" "nw-ap02" "nw-ap03" "nw-ap04" "nw-ap05" "nw-ap06" "nw-ap07"</t>
+          <t>['nw-ap01', 'nw-ap02', 'nw-ap03', 'nw-ap04', 'nw-ap05', 'nw-ap06', 'nw-ap07']</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1699,7 +1916,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"Baulkham Hills Meraki APs"</t>
+          <t>Baulkham Hills Meraki APs</t>
         </is>
       </c>
     </row>
@@ -1714,7 +1931,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1767,7 +1984,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"DNS"</t>
+          <t>DNS</t>
         </is>
       </c>
     </row>
@@ -1779,7 +1996,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"HTTP"</t>
+          <t>HTTP</t>
         </is>
       </c>
     </row>
@@ -1791,7 +2008,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"HTTPS"</t>
+          <t>HTTPS</t>
         </is>
       </c>
     </row>
@@ -1803,12 +2020,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"IMAP"</t>
+          <t>IMAP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>"Email"</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -1820,12 +2037,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"IMAPS"</t>
+          <t>IMAPS</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>"Email"</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -1837,12 +2054,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"LDAP"</t>
+          <t>LDAP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>"Authentication"</t>
+          <t>Authentication</t>
         </is>
       </c>
     </row>
@@ -1859,7 +2076,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"DCE-RPC"</t>
+          <t>DCE-RPC</t>
         </is>
       </c>
     </row>
@@ -1871,12 +2088,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"POP3"</t>
+          <t>POP3</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>"Email"</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -1888,12 +2105,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"POP3S"</t>
+          <t>POP3S</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>"Email"</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -1905,7 +2122,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"SAMBA"</t>
+          <t>SAMBA</t>
         </is>
       </c>
     </row>
@@ -1917,12 +2134,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"SMTP"</t>
+          <t>SMTP</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>"Email"</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
@@ -1934,24 +2151,24 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"SMTPS"</t>
+          <t>SMTPS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>"Email"</t>
+          <t>Email</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" t="inlineStr">
         <is>
-          <t>"KERBEROS"</t>
+          <t>KERBEROS</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>"Authentication"</t>
+          <t>Authentication</t>
         </is>
       </c>
     </row>
@@ -1963,12 +2180,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"LDAP_UDP"</t>
+          <t>LDAP_UDP</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>"Authentication"</t>
+          <t>Authentication</t>
         </is>
       </c>
     </row>
@@ -1980,19 +2197,19 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"SMB"</t>
+          <t>SMB</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="C17" t="inlineStr">
         <is>
-          <t>"ALL"</t>
+          <t>ALL</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>"General"</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2004,12 +2221,12 @@
     <row r="18">
       <c r="C18" t="inlineStr">
         <is>
-          <t>"ALL_ICMP"</t>
+          <t>ALL_ICMP</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>"General"</t>
+          <t>General</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2031,14 +2248,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>"NTP"</t>
+          <t>NTP</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="C20" t="inlineStr">
         <is>
-          <t>"PING"</t>
+          <t>PING</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2060,7 +2277,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"SNMP"</t>
+          <t>SNMP</t>
         </is>
       </c>
     </row>
@@ -2072,7 +2289,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>"SSH"</t>
+          <t>SSH</t>
         </is>
       </c>
     </row>
@@ -2084,7 +2301,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>"TRACEROUTE"</t>
+          <t>TRACEROUTE</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2313,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>"webproxy"</t>
+          <t>webproxy</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -2118,7 +2335,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"FortiGateAdminPort"</t>
+          <t>FortiGateAdminPort</t>
         </is>
       </c>
     </row>
@@ -2130,7 +2347,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"TACACS+"</t>
+          <t>TACACS+</t>
         </is>
       </c>
     </row>
@@ -2142,7 +2359,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"udp-443"</t>
+          <t>udp-443</t>
         </is>
       </c>
     </row>
@@ -2154,7 +2371,19 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>"tcp-8080"</t>
+          <t>tcp-8080</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>7351</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Meraki Ports</t>
         </is>
       </c>
     </row>
@@ -2180,7 +2409,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>member</t>
+          <t>members</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -2192,48 +2421,48 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>"DNS" "IMAP" "IMAPS" "POP3" "POP3S" "SMTP" "SMTPS"</t>
+          <t>['DNS', 'IMAP', 'IMAPS', 'POP3', 'POP3S', 'SMTP', 'SMTPS']</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>"Email Access"</t>
+          <t>Email Access</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>"DNS" "HTTP" "HTTPS"</t>
+          <t>['DNS', 'HTTP', 'HTTPS']</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>"Web Access"</t>
+          <t>Web Access</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>"DCE-RPC" "DNS" "KERBEROS" "LDAP" "LDAP_UDP" "SAMBA" "SMB"</t>
+          <t>['DCE-RPC', 'DNS', 'KERBEROS', 'LDAP', 'LDAP_UDP', 'SAMBA', 'SMB']</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>"Windows AD"</t>
+          <t>Windows AD</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>"DCE-RPC" "DNS" "HTTPS"</t>
+          <t>['DCE-RPC', 'DNS', 'HTTPS']</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>"Exchange Server"</t>
+          <t>Exchange Server</t>
         </is>
       </c>
     </row>
@@ -2341,12 +2570,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>"ALL_ICMP" "FortiGateAdminPort" "HTTPS" "SNMP" "SSH"</t>
+          <t>['ALL_ICMP', 'FortiGateAdminPort', 'HTTPS', 'SNMP', 'SSH']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2356,22 +2585,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>"NetSG SNCK Loopback Allocation"</t>
+          <t>['NetSG', 'SNCK', 'Loopback', 'Allocation']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>"NetSG Mgmt DMZ Subnets"</t>
+          <t>['NetSG', 'Mgmt', 'DMZ', 'Subnets']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>"loopback0" "internal3"</t>
+          <t>['loopback0', 'internal3']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>"Zone_IPWan"</t>
+          <t>['Zone_IPWan']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -2381,7 +2610,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>"NetSG Management Inbound"</t>
+          <t>NetSG Management Inbound</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -2398,12 +2627,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>"NTP"</t>
+          <t>['NTP']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2413,22 +2642,22 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>"NetSG NTP Servers"</t>
+          <t>['NetSG', 'NTP', 'Servers']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>"NetSG SNCK Loopback Allocation"</t>
+          <t>['NetSG', 'SNCK', 'Loopback', 'Allocation']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>"Zone_IPWan"</t>
+          <t>['Zone_IPWan']</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>"loopback0"</t>
+          <t>['loopback0']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -2438,7 +2667,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>"NetSG NTP Servers"</t>
+          <t>NetSG NTP Servers</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -2455,12 +2684,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>"TACACS+"</t>
+          <t>['TACACS+']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2470,22 +2699,22 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>"NetSG Tacacs Servers"</t>
+          <t>['NetSG', 'Tacacs', 'Servers']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>"NetSG SNCK Loopback Allocation"</t>
+          <t>['NetSG', 'SNCK', 'Loopback', 'Allocation']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>"Zone_IPWan"</t>
+          <t>['Zone_IPWan']</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>"loopback0"</t>
+          <t>['loopback0']</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -2495,7 +2724,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>"NetSG TACACS Servers"</t>
+          <t>NetSG TACACS Servers</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -2512,12 +2741,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>"PING" "TRACEROUTE"</t>
+          <t>['PING', 'TRACEROUTE']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2527,22 +2756,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>"Private Address Spaces"</t>
+          <t>['Private', 'Address', 'Spaces']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>"Private Address Spaces"</t>
+          <t>['Private', 'Address', 'Spaces']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>"any"</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>"any"</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -2552,7 +2781,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>"Trusted Internal ICMP"</t>
+          <t>Trusted Internal ICMP</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -2569,12 +2798,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>"ALL"</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2584,22 +2813,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>"Zone_IPWan"</t>
+          <t>['Zone_IPWan']</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>"Zone_Data"</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -2609,7 +2838,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>"LAN to IPWAN"</t>
+          <t>LAN to IPWAN</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -2626,12 +2855,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>"ALL"</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2641,22 +2870,22 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>"Zone_Data"</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>"Zone_IPWan"</t>
+          <t>['Zone_IPWan']</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -2666,7 +2895,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>"IPWAN to LAN"</t>
+          <t>IPWAN to LAN</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -2683,32 +2912,32 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>"ALL"</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>"Private Address Spaces"</t>
+          <t>['Private', 'Address', 'Spaces']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>"virtual-wan-link"</t>
+          <t>['virtual-wan-link']</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>"any"</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -2718,7 +2947,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>"Protect Internal"</t>
+          <t>Protect Internal</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -2735,12 +2964,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>"Meraki Ports" "PING" "NTP"</t>
+          <t>['Meraki', 'Ports', 'PING', 'NTP']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2750,22 +2979,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>"Baulkham Hills Meraki APs"</t>
+          <t>['Baulkham', 'Hills', 'Meraki', 'APs']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>"virtual-wan-link"</t>
+          <t>['virtual-wan-link']</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>"Zone_Data"</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -2775,7 +3004,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>"Meraki Access Points"</t>
+          <t>Meraki Access Points</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -2790,12 +3019,12 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>"This is only additional ports required for Speedtest.net.</t>
+          <t>This is only additional ports required for Speedtest.net.</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>"certificate-inspection"</t>
+          <t>certificate-inspection</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -2812,12 +3041,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>"udp-443" "tcp-8080"</t>
+          <t>['udp-443', 'tcp-8080']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -2827,22 +3056,22 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>"virtual-wan-link"</t>
+          <t>['virtual-wan-link']</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>"Zone_Data"</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -2852,7 +3081,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>"Speedtest Access"</t>
+          <t>Speedtest Access</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -2867,12 +3096,12 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>"This is only additional ports required for Speedtest.net.</t>
+          <t>This is only additional ports required for Speedtest.net.</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>"certificate-inspection"</t>
+          <t>certificate-inspection</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -2889,12 +3118,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>"ALL"</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -2904,22 +3133,22 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>"virtual-wan-link"</t>
+          <t>['virtual-wan-link']</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>"Zone_Data"</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -2929,7 +3158,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>"General Internet Access"</t>
+          <t>General Internet Access</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -2944,7 +3173,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>"certificate-inspection"</t>
+          <t>certificate-inspection</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -2961,32 +3190,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>"ALL"</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"always"</t>
+          <t>always</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>"all"</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>"any"</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>"any"</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -2996,7 +3225,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>"Deny and Log"</t>
+          <t>Deny and Log</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -3059,7 +3288,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10.0.0.0 255.0.0.0</t>
+          <t>10.0.0.0/8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3081,7 +3310,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>100.64.0.0 255.192.0.0</t>
+          <t>100.64.0.0/10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3103,7 +3332,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>172.16.0.0 255.240.0.0</t>
+          <t>172.16.0.0/12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3125,7 +3354,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>192.168.0.0 255.255.0.0</t>
+          <t>192.168.0.0/16</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3149,7 +3378,7 @@
     <row r="7">
       <c r="C7" t="inlineStr">
         <is>
-          <t>192.168.6.0 255.255.255.0</t>
+          <t>192.168.6.0/24</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3161,7 +3390,7 @@
     <row r="8">
       <c r="C8" t="inlineStr">
         <is>
-          <t>192.168.7.0 255.255.255.0</t>
+          <t>192.168.7.0/24</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -3173,7 +3402,7 @@
     <row r="9">
       <c r="C9" t="inlineStr">
         <is>
-          <t>103.99.241.36 255.255.255.255</t>
+          <t>103.99.241.36/32</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -3190,7 +3419,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>103.99.241.35 255.255.255.255</t>
+          <t>103.99.241.35/32</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -3202,7 +3431,7 @@
     <row r="11">
       <c r="C11" t="inlineStr">
         <is>
-          <t>103.99.243.129 255.255.255.255</t>
+          <t>103.99.243.129/32</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -3214,7 +3443,7 @@
     <row r="12">
       <c r="C12" t="inlineStr">
         <is>
-          <t>103.99.241.10 255.255.255.255</t>
+          <t>103.99.241.10/32</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">

</xml_diff>

<commit_message>
clean up sample config and added more context into readme
</commit_message>
<xml_diff>
--- a/outputs/configuration.xlsx
+++ b/outputs/configuration.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,11 @@
           <t>device-identification</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ipv6</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1067,278 +1072,9 @@
           <t>enable</t>
         </is>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>wan</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>['ping']</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>dia2</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>89.147.120.215/31</t>
-        </is>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>lan</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>['ping']</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>ipwan2</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>100.66.11.26/30</t>
-        </is>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>wan</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>fext-wan</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>fex1</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>dhcp</t>
-        </is>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>tunnel</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>['ping']</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>au02-vp-02</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>100.66.11.134/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>tunnel</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>['ping']</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>au04-vp-01</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>100.66.11.166/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>lan</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>aggregate</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>['ping']</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>lag0</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>192.168.5.1/24</t>
-        </is>
-      </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>['internal1', 'internal2']</t>
-        </is>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>wan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>['ping']</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>root</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>dia1</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>89.147.120.213/31</t>
-        </is>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>enable</t>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>{'ip6-address': 'fec0::0003:209:0fff:fe83:25c7/64'}</t>
         </is>
       </c>
     </row>
@@ -1353,7 +1089,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1379,26 +1115,6 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>end_ip</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>start_ip</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>associated-interface</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>subnet</t>
         </is>
       </c>
@@ -1447,353 +1163,185 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>154d08b4-c6bd-51ec-61c0-b9ff10463e07</t>
+          <t>9dd63474-c17e-51ec-414e-d391de278269</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SSLVPN_TUNNEL_ADDR1</t>
+          <t>Private RFC1918 10.0.0.0</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10.212.134.210</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10.212.134.200</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>ssl.root</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>iprange</t>
+          <t>10.0.0.0/8</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17ed18fa-c7c3-51ec-50c1-c283f73dbe8c</t>
+          <t>accc70ba-c17e-51ec-a150-34dd5295486c</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FCTEMS_ALL_FORTICLOUD_SERVERS</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>dynamic</t>
+          <t>Private RFC1918 172.16.0.0</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>172.16.0.0/12</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>9dd63474-c17e-51ec-414e-d391de278269</t>
+          <t>bacc7c8c-c17e-51ec-1b44-78ac0eaac98d</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Private RFC1918 10.0.0.0</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>10.0.0.0/8</t>
+          <t>Private RFC1918 192.168.0.0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>192.168.0.0/16</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>accc70ba-c17e-51ec-a150-34dd5295486c</t>
+          <t>f4c6c104-c17e-51ec-79d7-995927036c68</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Private RFC1918 172.16.0.0</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>172.16.0.0/12</t>
+          <t>Private RFC6598 100.64.0.0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>100.64.0.0/10</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>bacc7c8c-c17e-51ec-1b44-78ac0eaac98d</t>
+          <t>ea5b02fe-e87d-51ec-45de-1058c8dc3015</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Private RFC1918 192.168.0.0</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>192.168.0.0/16</t>
+          <t>nw-ap01</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>192.168.7.10/32</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>f4c6c104-c17e-51ec-79d7-995927036c68</t>
+          <t>f55a2360-e87d-51ec-a5d9-f95c9392cb67</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Private RFC6598 100.64.0.0</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>100.64.0.0/10</t>
+          <t>nw-ap02</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>192.168.7.11/32</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>7193e550-c17e-51ec-5133-435ce1ae000e</t>
+          <t>017a06d8-e87e-51ec-ab97-93410a582ec4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>NetSG AU01 Mgmt DMZ Subnet</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>100.68.1.0/24</t>
+          <t>nw-ap03</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>192.168.7.13/32</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>7e302878-c17e-51ec-2aaa-add873a5d0b5</t>
+          <t>0ba7bf88-e87e-51ec-76cc-c7cc7b08155b</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>NetSG AU02 Mgmt DMZ Subnet</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>100.68.2.0/24</t>
+          <t>nw-ap04</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>192.168.7.14/32</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>061f6e06-c17f-51ec-9ace-68cf37c88867</t>
+          <t>17a955da-e87e-51ec-e257-f807bbfdb39b</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NetSG NTP Server 1</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>103.74.171.50/32</t>
+          <t>nw-ap05</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>192.168.7.15/32</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>10262f7a-c17f-51ec-423e-2abd67c5a3e0</t>
+          <t>265076fe-e87e-51ec-ecc0-4471a7f569c0</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NetSG NTP Server 2</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>103.99.241.50/32</t>
+          <t>nw-ap06</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>192.168.7.16/32</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>8f652b66-c17e-51ec-d179-d72dbd46e0e5</t>
+          <t>2e109428-e87e-51ec-6083-96f05f3296af</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>NetSG SNCK Loopback Allocation</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>100.64.24.0/24</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>19948d0e-c17f-51ec-208d-651c24467a49</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>NetSG Tacacs Server 1</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>100.68.1.133/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2353eaf6-c17f-51ec-935d-653521fb65a3</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>NetSG Tacacs Server 2</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>100.68.2.133/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>ea5b02fe-e87d-51ec-45de-1058c8dc3015</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>nw-ap01</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>192.168.7.10/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>f55a2360-e87d-51ec-a5d9-f95c9392cb67</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>nw-ap02</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>192.168.7.11/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>017a06d8-e87e-51ec-ab97-93410a582ec4</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>nw-ap03</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>192.168.7.13/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>0ba7bf88-e87e-51ec-76cc-c7cc7b08155b</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>nw-ap04</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>192.168.7.14/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>17a955da-e87e-51ec-e257-f807bbfdb39b</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>nw-ap05</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>192.168.7.15/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>265076fe-e87e-51ec-ecc0-4471a7f569c0</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>nw-ap06</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>192.168.7.16/32</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2e109428-e87e-51ec-6083-96f05f3296af</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
           <t>nw-ap07</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>192.168.7.17/32</t>
         </is>
@@ -1810,7 +1358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1838,7 +1386,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>['Private', 'RFC1918', '10.0.0.0', 'Private', 'RFC1918', '172.16.0.0', 'Private', 'RFC1918', '192.168.0.0', 'Private', 'RFC6598', '100.64.0.0']</t>
+          <t>Private</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1855,68 +1403,187 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>['NetSG', 'AU01', 'Mgmt', 'DMZ', 'Subnet', 'NetSG', 'AU02', 'Mgmt', 'DMZ', 'Subnet']</t>
+          <t>RFC1918</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3d04fc60-c17f-51ec-0e13-e7a73304a5ed</t>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NetSG Mgmt DMZ Subnets</t>
+          <t>Private Address Spaces</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>['NetSG', 'NTP', 'Server', '1', 'NetSG', 'NTP', 'Server', '2']</t>
+          <t>10.0.0.0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>52ed8bdc-c17f-51ec-8732-eb6bb4f3e18c</t>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NetSG NTP Servers</t>
+          <t>Private Address Spaces</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>['NetSG', 'Tacacs', 'Server', '1', 'NetSG', 'Tacacs', 'Server', '2']</t>
+          <t>Private</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>602507bc-c17f-51ec-b284-494cdbd261c2</t>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NetSG Tacacs Servers</t>
+          <t>Private Address Spaces</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>['nw-ap01', 'nw-ap02', 'nw-ap03', 'nw-ap04', 'nw-ap05', 'nw-ap06', 'nw-ap07']</t>
+          <t>RFC1918</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3e2be308-e87e-51ec-ecb0-49a688dc1ce9</t>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Baulkham Hills Meraki APs</t>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>172.16.0.0</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RFC1918</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>192.168.0.0</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Private</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RFC6598</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>100.64.0.0</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>49e6e57e-c17f-51ec-586d-dff4be338514</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Private Address Spaces</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2144,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2570,7 +2237,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['ALL_ICMP', 'FortiGateAdminPort', 'HTTPS', 'SNMP', 'SSH']</t>
+          <t>['PING', 'TRACEROUTE']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2585,37 +2252,37 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['NetSG', 'SNCK', 'Loopback', 'Allocation']</t>
+          <t>['Private', 'Address', 'Spaces']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['NetSG', 'Mgmt', 'DMZ', 'Subnets']</t>
+          <t>['Private', 'Address', 'Spaces']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>['loopback0', 'internal3']</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['Zone_IPWan']</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>652c632c-c23d-51ec-9b0c-366b86d43aa6</t>
+          <t>6530c480-c23d-51ec-65f0-49633702aa26</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NetSG Management Inbound</t>
+          <t>Trusted Internal ICMP</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2294,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['NTP']</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2642,12 +2309,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['NetSG', 'NTP', 'Servers']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['NetSG', 'SNCK', 'Loopback', 'Allocation']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2657,22 +2324,22 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['loopback0']</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>652fad48-c23d-51ec-b6f9-837c0a35e74b</t>
+          <t>65314c98-c23d-51ec-3c19-dbed9849c03f</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NetSG NTP Servers</t>
+          <t>LAN to IPWAN</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
     </row>
@@ -2684,7 +2351,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['TACACS+']</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2699,37 +2366,37 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['NetSG', 'Tacacs', 'Servers']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['NetSG', 'SNCK', 'Loopback', 'Allocation']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>['Zone_Data']</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
           <t>['Zone_IPWan']</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>['loopback0']</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>653036be-c23d-51ec-98c9-1e91fe7e21f6</t>
+          <t>6531d5c8-c23d-51ec-38ed-d0fdd6ee45ba</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>NetSG TACACS Servers</t>
+          <t>IPWAN to LAN</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2408,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['PING', 'TRACEROUTE']</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2749,11 +2416,6 @@
           <t>always</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>accept</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>['Private', 'Address', 'Spaces']</t>
@@ -2761,32 +2423,32 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['Private', 'Address', 'Spaces']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>['virtual-wan-link']</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>['any']</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>['any']</t>
-        </is>
-      </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>6530c480-c23d-51ec-65f0-49633702aa26</t>
+          <t>4674fb24-e871-51ec-f6d9-123c05f4aa93</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Trusted Internal ICMP</t>
+          <t>Protect Internal</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>11</t>
         </is>
       </c>
     </row>
@@ -2798,7 +2460,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['ALL']</t>
+          <t>['Meraki', 'Ports', 'PING', 'NTP']</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -2818,12 +2480,12 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['all']</t>
+          <t>['Baulkham', 'Hills', 'Meraki', 'APs']</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>['Zone_IPWan']</t>
+          <t>['virtual-wan-link']</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -2833,17 +2495,37 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>65314c98-c23d-51ec-3c19-dbed9849c03f</t>
+          <t>476097d0-e87d-51ec-bf3a-e97a6bcbeef4</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>LAN to IPWAN</t>
+          <t>Meraki Access Points</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>This is only additional ports required for Speedtest.net.</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>certificate-inspection</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>enable</t>
         </is>
       </c>
     </row>
@@ -2855,7 +2537,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['ALL']</t>
+          <t>['udp-443', 'tcp-8080']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2880,27 +2562,47 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>['virtual-wan-link']</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>['Zone_Data']</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>['Zone_IPWan']</t>
-        </is>
-      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>6531d5c8-c23d-51ec-38ed-d0fdd6ee45ba</t>
+          <t>95857f32-e870-51ec-38d8-9faf909dc008</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>IPWAN to LAN</t>
+          <t>Speedtest Access</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>This is only additional ports required for Speedtest.net.</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>certificate-inspection</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>enable</t>
         </is>
       </c>
     </row>
@@ -2920,9 +2622,14 @@
           <t>always</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>accept</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['Private', 'Address', 'Spaces']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2937,22 +2644,37 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>['any']</t>
+          <t>['Zone_Data']</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>4674fb24-e871-51ec-f6d9-123c05f4aa93</t>
+          <t>6532647a-c23d-51ec-afcf-59860ca87a75</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Protect Internal</t>
+          <t>General Internet Access</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>enable</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>certificate-inspection</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>enable</t>
         </is>
       </c>
     </row>
@@ -2964,7 +2686,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['Meraki', 'Ports', 'PING', 'NTP']</t>
+          <t>['ALL']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -2972,11 +2694,6 @@
           <t>always</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>accept</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>['all']</t>
@@ -2984,251 +2701,30 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>['Baulkham', 'Hills', 'Meraki', 'APs']</t>
+          <t>['all']</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>['virtual-wan-link']</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>['Zone_Data']</t>
+          <t>['any']</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>476097d0-e87d-51ec-bf3a-e97a6bcbeef4</t>
+          <t>73129d2e-c645-51ec-7001-bbead48d8665</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Meraki Access Points</t>
+          <t>Deny and Log</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>This is only additional ports required for Speedtest.net.</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>certificate-inspection</t>
-        </is>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>all</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>['udp-443', 'tcp-8080']</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>accept</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>['all']</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>['all']</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>['virtual-wan-link']</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>['Zone_Data']</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>95857f32-e870-51ec-38d8-9faf909dc008</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Speedtest Access</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>This is only additional ports required for Speedtest.net.</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>certificate-inspection</t>
-        </is>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>all</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>['ALL']</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>accept</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>['all']</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>['all']</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>['virtual-wan-link']</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>['Zone_Data']</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>6532647a-c23d-51ec-afcf-59860ca87a75</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>General Internet Access</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>certificate-inspection</t>
-        </is>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>enable</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>all</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>['ALL']</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>['all']</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>['all']</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>['any']</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>['any']</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>73129d2e-c645-51ec-7001-bbead48d8665</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Deny and Log</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
         <is>
           <t>8</t>
         </is>

</xml_diff>